<commit_message>
Arreglos sugerencias de Ruben
</commit_message>
<xml_diff>
--- a/Libros/pobrezaCSV.xlsx
+++ b/Libros/pobrezaCSV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="1_01" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -60,22 +60,13 @@
     <t>Pobreza extrema</t>
   </si>
   <si>
-    <t>De 0 a 4</t>
-  </si>
-  <si>
-    <t>De 5 a 9</t>
-  </si>
-  <si>
-    <t>De 10 a 14</t>
-  </si>
-  <si>
-    <t>De 15 a 17</t>
-  </si>
-  <si>
     <t>De 0 a 17</t>
   </si>
   <si>
-    <t>Entre 18 y 19</t>
+    <t>De 0 a 9</t>
+  </si>
+  <si>
+    <t>De 10 a 17</t>
   </si>
 </sst>
 </file>
@@ -295,7 +286,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -334,12 +325,12 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A2:A23 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A2:B2 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -409,13 +400,13 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="A2:B2 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -622,12 +613,12 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A2:A23 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -684,12 +675,12 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A2:A23 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -746,13 +737,13 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -959,12 +950,12 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A2:A23 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1021,13 +1012,13 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1231,10 +1222,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B65536"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1256,7 +1247,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="21" t="n">
-        <v>70.1138131411546</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="21" t="n">
-        <v>70.3386269988124</v>
+        <v>70.2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,41 +1263,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="21" t="n">
-        <v>67.3464227240395</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="21" t="n">
-        <v>63.4863212160658</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="21" t="n">
-        <v>68.2225355103856</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="21" t="n">
-        <v>58.860187497789</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>65.9</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1326,12 +1292,12 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,13 +1502,13 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,12 +1714,12 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A2:A23 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A2:B2 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1810,7 +1776,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="A2:A23 B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="A2:B2 B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1898,12 +1864,12 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1973,13 +1939,13 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A2:A23 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A2:B2 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2185,13 +2151,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A2:A23 B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2249,12 +2215,12 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2311,14 +2277,14 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2388,12 +2354,12 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>